<commit_message>
added many admin features
</commit_message>
<xml_diff>
--- a/src/static/questions/demo.xlsx
+++ b/src/static/questions/demo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="103">
   <si>
     <t>question_no</t>
   </si>
@@ -124,7 +124,268 @@
     <t>Foreign Deposit Insurance Corporation</t>
   </si>
   <si>
-    <t/>
+    <t>FDIC can reimburse personal and business accounts  only upto $_______  invested in a bank.</t>
+  </si>
+  <si>
+    <r>
+      <t/>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">__________ was the largest bank failure in the past upto 2016. </t>
+    </r>
+  </si>
+  <si>
+    <t>Wachovia</t>
+  </si>
+  <si>
+    <t>Bank of America</t>
+  </si>
+  <si>
+    <t>MetWest Bank</t>
+  </si>
+  <si>
+    <t>Washington Mutual</t>
+  </si>
+  <si>
+    <t>The significant bank failure amongst the 2023 bank failures is ______.</t>
+  </si>
+  <si>
+    <t>Signature Bank Failure</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sillicon Valley Bank Failure</t>
+  </si>
+  <si>
+    <t>First Republic Bank  Failure</t>
+  </si>
+  <si>
+    <t>Washington Federal Bank for Savings  Failure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FDIC’s biggest worry in Sillicon Valley Bank crisis is __________. </t>
+  </si>
+  <si>
+    <t>The impact on the tech industry</t>
+  </si>
+  <si>
+    <t>The loss of confidence in the banking system.</t>
+  </si>
+  <si>
+    <t>They couldn’t find a buyer in shorter time</t>
+  </si>
+  <si>
+    <t>he impact on the global financial system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the future the bank’s contribution to FDIC ________. </t>
+  </si>
+  <si>
+    <t>May go up</t>
+  </si>
+  <si>
+    <t>May go down</t>
+  </si>
+  <si>
+    <t>May remain the same</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May be abolished </t>
+  </si>
+  <si>
+    <t>May go up.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The interviewer in the conversation, J.R.Whalen  is working at  __________.  </t>
+  </si>
+  <si>
+    <t>The New York Times</t>
+  </si>
+  <si>
+    <r>
+      <t/>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Washington Post</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF1f1f1f"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>The Wall Street Journal</t>
+  </si>
+  <si>
+    <t>USA Today</t>
+  </si>
+  <si>
+    <t>Wall Street Journal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The interviewee of the conversation is  columnist named  _________. </t>
+  </si>
+  <si>
+    <t>David Brooks</t>
+  </si>
+  <si>
+    <t>Callum Borchers</t>
+  </si>
+  <si>
+    <t>Callum Brothers</t>
+  </si>
+  <si>
+    <t>Maureen Dowd</t>
+  </si>
+  <si>
+    <t>Deloitte’s survey found that young workers admire their ______ who can balance work and life.</t>
+  </si>
+  <si>
+    <t>Colleagues</t>
+  </si>
+  <si>
+    <t>Companions</t>
+  </si>
+  <si>
+    <t>Peers</t>
+  </si>
+  <si>
+    <t>Subordinates</t>
+  </si>
+  <si>
+    <t>However, the same individuals thought their most important identity in life is their __________ than hobbies or fashion.</t>
+  </si>
+  <si>
+    <t>Work</t>
+  </si>
+  <si>
+    <t>Personal relationships</t>
+  </si>
+  <si>
+    <t>Health and wellness</t>
+  </si>
+  <si>
+    <t>Spirituality</t>
+  </si>
+  <si>
+    <t>Jobs</t>
+  </si>
+  <si>
+    <t>Work-life balance is something that is unfortunately _____ to say than to practice. Easier</t>
+  </si>
+  <si>
+    <t>Easier</t>
+  </si>
+  <si>
+    <t>Tougher</t>
+  </si>
+  <si>
+    <t>Difficult</t>
+  </si>
+  <si>
+    <t>Different</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Catherine Smith Lakari literally carries around a card that says _________ in her wallet. </t>
+  </si>
+  <si>
+    <t>Lifestyle balance</t>
+  </si>
+  <si>
+    <t>Mindfulness</t>
+  </si>
+  <si>
+    <t>Me-time</t>
+  </si>
+  <si>
+    <t>Work-life balance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Doing it for the gram” refers to posting serene personal life photos in ________. </t>
+  </si>
+  <si>
+    <t>Instagram</t>
+  </si>
+  <si>
+    <t>Pinterest</t>
+  </si>
+  <si>
+    <t>TikTok</t>
+  </si>
+  <si>
+    <t>Snapchat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The second bucket of inspiring people for youngsters are senior worker or boss who exudes the image  of _______. </t>
+  </si>
+  <si>
+    <t>Living the dream</t>
+  </si>
+  <si>
+    <t>Having your cake and eating it too</t>
+  </si>
+  <si>
+    <t>Have it all</t>
+  </si>
+  <si>
+    <t>Ticking all the boxes</t>
+  </si>
+  <si>
+    <t>_________ is the main reason from maintaining work-life balance young professionals want.</t>
+  </si>
+  <si>
+    <t>Hustle Culture</t>
+  </si>
+  <si>
+    <t>Burnout culture</t>
+  </si>
+  <si>
+    <t>Grind culture</t>
+  </si>
+  <si>
+    <t>Rat race</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Managers who want hard workers now do hiring _______ instead of Millennials and Gen Z. </t>
+  </si>
+  <si>
+    <t>iGen</t>
+  </si>
+  <si>
+    <t>Zoomers</t>
+  </si>
+  <si>
+    <t>Older people</t>
+  </si>
+  <si>
+    <t>Younger people</t>
   </si>
 </sst>
 </file>
@@ -435,7 +696,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="29">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -479,46 +740,31 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="3" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="15" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="15" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="18" applyBorder="1" fontId="4" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="18" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="19" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="19" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -529,6 +775,9 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -841,15 +1090,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="29" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="30" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="30" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="30" width="98.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="31" width="40.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="31" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="31" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="31" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="32" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="24" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="25" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="25" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="25" width="98.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="26" width="40.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="26" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="27" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="28" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -1003,338 +1252,378 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="8"/>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>29</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="13"/>
+      <c r="E7" s="10">
+        <v>250000</v>
+      </c>
+      <c r="F7" s="10">
+        <v>2500000</v>
+      </c>
+      <c r="G7" s="10">
+        <v>20500000</v>
+      </c>
+      <c r="H7" s="10">
+        <v>250000000</v>
+      </c>
+      <c r="I7" s="13">
+        <v>250000</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="8"/>
-      <c r="B8" s="16" t="s">
-        <v>29</v>
+      <c r="A8" s="8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
-      <c r="E8" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>29</v>
+      <c r="E8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>34</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="8"/>
-      <c r="B9" s="15" t="s">
-        <v>29</v>
+      <c r="A9" s="8">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>35</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
-      <c r="E9" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="I9" s="19" t="s">
-        <v>29</v>
+      <c r="E9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>37</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="8"/>
-      <c r="B10" s="15" t="s">
-        <v>29</v>
+      <c r="A10" s="8">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>40</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
-      <c r="E10" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="I10" s="19" t="s">
-        <v>29</v>
+      <c r="E10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>43</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="8"/>
-      <c r="B11" s="15" t="s">
-        <v>29</v>
+      <c r="A11" s="8">
+        <v>10</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
-      <c r="E11" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="I11" s="19" t="s">
-        <v>29</v>
+      <c r="E11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>50</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="8"/>
-      <c r="B12" s="15" t="s">
-        <v>29</v>
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>51</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
-      <c r="E12" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="I12" s="20" t="s">
-        <v>29</v>
+      <c r="E12" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>56</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="8"/>
-      <c r="B13" s="15" t="s">
-        <v>29</v>
+      <c r="A13" s="8">
+        <v>12</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
-      <c r="E13" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="I13" s="21" t="s">
-        <v>29</v>
+      <c r="E13" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>59</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="8"/>
-      <c r="B14" s="15" t="s">
-        <v>29</v>
+      <c r="A14" s="8">
+        <v>13</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>62</v>
       </c>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
-      <c r="E14" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="G14" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="H14" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="I14" s="21" t="s">
-        <v>29</v>
+      <c r="E14" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>65</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="8"/>
-      <c r="B15" s="15" t="s">
-        <v>29</v>
+      <c r="A15" s="8">
+        <v>14</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>67</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
-      <c r="E15" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="G15" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="H15" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="I15" s="21" t="s">
-        <v>29</v>
+      <c r="E15" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>72</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="8"/>
-      <c r="B16" s="15" t="s">
-        <v>29</v>
+      <c r="A16" s="8">
+        <v>15</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>73</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
-      <c r="E16" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="G16" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="I16" s="21" t="s">
-        <v>29</v>
+      <c r="E16" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I16" s="17" t="s">
+        <v>74</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="8"/>
-      <c r="B17" s="15" t="s">
-        <v>29</v>
+      <c r="A17" s="8">
+        <v>16</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
-      <c r="E17" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="G17" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="H17" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="I17" s="21" t="s">
-        <v>29</v>
+      <c r="E17" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>82</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="8"/>
-      <c r="B18" s="15" t="s">
-        <v>29</v>
+      <c r="A18" s="8">
+        <v>17</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>83</v>
       </c>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
-      <c r="E18" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="G18" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="H18" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="I18" s="21" t="s">
-        <v>29</v>
+      <c r="E18" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>84</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="8"/>
-      <c r="B19" s="15" t="s">
-        <v>29</v>
+      <c r="A19" s="8">
+        <v>18</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>88</v>
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
-      <c r="E19" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="H19" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="I19" s="21" t="s">
-        <v>29</v>
+      <c r="E19" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>91</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="8"/>
-      <c r="B20" s="15" t="s">
-        <v>29</v>
+      <c r="A20" s="8">
+        <v>19</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>93</v>
       </c>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
-      <c r="E20" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="F20" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="G20" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="H20" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="I20" s="21" t="s">
-        <v>29</v>
+      <c r="E20" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>94</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="23"/>
-      <c r="B21" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="F21" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="G21" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="H21" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="I21" s="21" t="s">
-        <v>29</v>
+      <c r="A21" s="19">
+        <v>20</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="H21" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>